<commit_message>
Penambahan dan Perbaikan Laporan Rekap Bulanan
Perbaikan kolom pada laporan TDI
Penambahan menu laporan untuk SIKP
</commit_message>
<xml_diff>
--- a/saved/laporan_situ.xlsx
+++ b/saved/laporan_situ.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="391">
   <si>
     <t>PEMERINTAH KABUPATEN BIREUEN</t>
   </si>
@@ -995,6 +995,42 @@
     <t>10 Januari 2018</t>
   </si>
   <si>
+    <t>510.1/0060/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>HAMDANI HUSIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "SURYA BARU TDR"</t>
+  </si>
+  <si>
+    <t>Jl. B. Aceh - Medan Gp. Bireuen Meunasah Capa</t>
+  </si>
+  <si>
+    <t>Dagang Bahan Bangunan</t>
+  </si>
+  <si>
+    <t>09 November 2017</t>
+  </si>
+  <si>
+    <t>510.1/0059/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>JAFAR ISHAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "METRO TANI"</t>
+  </si>
+  <si>
+    <t>Jl. Jangka Dsn. Suka Mulia Gp. Geundot</t>
+  </si>
+  <si>
+    <t>JANGKA</t>
+  </si>
+  <si>
+    <t>11 Februari 2018</t>
+  </si>
+  <si>
     <t>510.1/0061/KPPTSP/2015</t>
   </si>
   <si>
@@ -1008,6 +1044,135 @@
   </si>
   <si>
     <t>08 Februari 2018</t>
+  </si>
+  <si>
+    <t>510.1/0062/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>HAMZAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "UD. DARA DITA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gp. Jarommah Baroh</t>
+  </si>
+  <si>
+    <t>26 Januari 2015</t>
+  </si>
+  <si>
+    <t>25 Januari 2018</t>
+  </si>
+  <si>
+    <t>510.1/0063/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>MUSTAHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "CV. COBRA JAYA"</t>
+  </si>
+  <si>
+    <t>Jl. B. Aceh - Medan Gp. Matang Sagoe</t>
+  </si>
+  <si>
+    <t>01 Februari 2018</t>
+  </si>
+  <si>
+    <t>510.1/0064/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>MUNAWIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "CV. JULI RAYA"</t>
+  </si>
+  <si>
+    <t>Jl. Takengon Km. 6 Gp. Blang Keutumba</t>
+  </si>
+  <si>
+    <t>510.1/0067/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>MUTTAQIN, S.Farm, Apt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "APOTIK JAKARTA"</t>
+  </si>
+  <si>
+    <t>27 Januari 2015</t>
+  </si>
+  <si>
+    <t>510.1/0065/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "KAYLA BUTIK ONLINE"</t>
+  </si>
+  <si>
+    <t>Jualan Pakaian Jadi</t>
+  </si>
+  <si>
+    <t>510.1/0066/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>SYAHRIL M. DAUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "PT. KONSTRUKSI BUMI NUSANTARA"</t>
+  </si>
+  <si>
+    <t>Jln. B. Aceh - Medan No. 20-21  Gp. Cot Gapu</t>
+  </si>
+  <si>
+    <t>15 November 2017</t>
+  </si>
+  <si>
+    <t>510.1/0068/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>ZULKIFLI IBRAHIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "CV. PRIMA KECANA"</t>
+  </si>
+  <si>
+    <t>Jl. B. Aceh - Medan Gp. Bandar Bireuen</t>
+  </si>
+  <si>
+    <t>28 September 2017</t>
+  </si>
+  <si>
+    <t>510.1/0069/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>NUZUL IHSAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "UD. PERMATA GAS"</t>
+  </si>
+  <si>
+    <t>Jl. Buket Teukuh Gp. Bukit Teukueh</t>
+  </si>
+  <si>
+    <t>28 Januari 2015</t>
+  </si>
+  <si>
+    <t>27 Januari 2018</t>
+  </si>
+  <si>
+    <t>510.1/0070/KPPTSP/2015</t>
+  </si>
+  <si>
+    <t>HAMZATUL IQBAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "TUNAS BARU SERVICE"</t>
+  </si>
+  <si>
+    <t>Jl. Sinar Peusangan No. 23  Gp. Keude Matang Glumpang Dua</t>
+  </si>
+  <si>
+    <t>Dagang Spare Part Honda dan Service</t>
   </si>
   <si>
     <t>Kepala Kantor Pelayanan Perizinan Terpadu Satu Pintu</t>
@@ -1467,10 +1632,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L65" sqref="L65"/>
+      <selection activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3523,16 +3688,16 @@
         <v>329</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>57</v>
+        <v>330</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>324</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9" t="s">
@@ -3540,29 +3705,403 @@
       </c>
       <c r="L65" s="9"/>
     </row>
-    <row r="68" spans="1:12">
-      <c r="H68" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="H69" t="s">
+    <row r="66" spans="1:12" customHeight="1" ht="30">
+      <c r="A66" s="7">
+        <v>58</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="H73" t="s">
+      <c r="C66" s="7" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="H74" t="s">
+      <c r="D66" s="7" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="H75" t="s">
+      <c r="E66" s="7" t="s">
         <v>335</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:12" customHeight="1" ht="30">
+      <c r="A67" s="7">
+        <v>59</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="1:12" customHeight="1" ht="30">
+      <c r="A68" s="7">
+        <v>60</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="J68" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="1:12" customHeight="1" ht="30">
+      <c r="A69" s="7">
+        <v>61</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="1:12" customHeight="1" ht="30">
+      <c r="A70" s="7">
+        <v>62</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:12" customHeight="1" ht="30">
+      <c r="A71" s="7">
+        <v>63</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+    </row>
+    <row r="72" spans="1:12" customHeight="1" ht="30">
+      <c r="A72" s="7">
+        <v>64</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="J72" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+    </row>
+    <row r="73" spans="1:12" customHeight="1" ht="30">
+      <c r="A73" s="7">
+        <v>65</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L73" s="9"/>
+    </row>
+    <row r="74" spans="1:12" customHeight="1" ht="30">
+      <c r="A74" s="7">
+        <v>66</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="1:12" customHeight="1" ht="30">
+      <c r="A75" s="7">
+        <v>67</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="J75" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+    </row>
+    <row r="76" spans="1:12" customHeight="1" ht="30">
+      <c r="A76" s="7">
+        <v>68</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="J76" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="H79" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="H80" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="H84" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="H85" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="H86" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>